<commit_message>
cap nhat lai checklist
</commit_message>
<xml_diff>
--- a/Document/checklist/HungND_SWP3191_CodingCheckList.xlsx
+++ b/Document/checklist/HungND_SWP3191_CodingCheckList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study Material\SWP391 - ki moi\phan cua nhom\Source Code\SWP391_SE1630-NET_Group1\Document\checklist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584B78B2-9CD8-46D6-9D68-81417685FFC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342F46E0-D7B8-4449-AD2E-5134D91DC93C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1035,7 +1035,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H42" sqref="H42"/>
+      <selection pane="bottomRight" activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1086,7 +1086,7 @@
         <v>90</v>
       </c>
       <c r="H2">
-        <v>90</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="2" customFormat="1" ht="17.25" customHeight="1">

</xml_diff>